<commit_message>
Proyek list by peneliti
</commit_message>
<xml_diff>
--- a/storage/exports/Laporan Keuangan 2018.xlsx
+++ b/storage/exports/Laporan Keuangan 2018.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="21">
   <si>
     <t>Laporan Keuangan Pusat Studi Biofarmaka Tropika LPPM IPB Tahun 2018</t>
   </si>
@@ -38,13 +38,46 @@
     <t>Saldo tanggal 31 Desember 2017</t>
   </si>
   <si>
+    <t>15-May-18</t>
+  </si>
+  <si>
+    <t>Ninik Lestari Ningsih; beli bahan kimia</t>
+  </si>
+  <si>
+    <t>Sistem Informasi Manajemen Penelitian</t>
+  </si>
+  <si>
+    <t>Giro PKU</t>
+  </si>
+  <si>
+    <t>9-Jun-18</t>
+  </si>
+  <si>
+    <t>Alifka Aditya Putra; Saldo Awal</t>
+  </si>
+  <si>
+    <t>The International Conference on Advanced Computer Science and Information System (ICACSIS)</t>
+  </si>
+  <si>
     <t>16-Jun-18</t>
   </si>
   <si>
     <t>Ninik Lestari Ningsih; Saldo awal Giro PKU</t>
   </si>
   <si>
-    <t>Giro PKU</t>
+    <t>17-Jun-18</t>
+  </si>
+  <si>
+    <t>Alifka Aditya Putra; Saldo Awal Rutin</t>
+  </si>
+  <si>
+    <t>Rutin</t>
+  </si>
+  <si>
+    <t>Ninik Lestari Ningsih; Saldo Awal LPSB</t>
+  </si>
+  <si>
+    <t>LPSB</t>
   </si>
 </sst>
 </file>
@@ -440,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -509,25 +542,120 @@
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8">
-        <v>100000000</v>
-      </c>
+      <c r="C5" s="8">
+        <v>50000</v>
+      </c>
+      <c r="D5" s="8"/>
       <c r="E5" s="8">
         <f>E4+C5-D5</f>
-        <v>-100000000</v>
+        <v>50000</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="2"/>
+    <row r="6" spans="1:6" customHeight="1" ht="15.75">
+      <c r="A6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8">
+        <v>50000</v>
+      </c>
+      <c r="E6" s="8">
+        <f>E5+C6-D6</f>
+        <v>0</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" customHeight="1" ht="15.75">
+      <c r="A7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4000</v>
+      </c>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8">
+        <f>E6+C7-D7</f>
+        <v>4000</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" customHeight="1" ht="15.75">
+      <c r="A8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8">
+        <v>100000000</v>
+      </c>
+      <c r="E8" s="8">
+        <f>E7+C8-D8</f>
+        <v>-99996000</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" customHeight="1" ht="15.75">
+      <c r="A9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="8">
+        <v>60000</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8">
+        <f>E8+C9-D9</f>
+        <v>-99936000</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" customHeight="1" ht="15.75">
+      <c r="A10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="8">
+        <v>500000000</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8">
+        <f>E9+C10-D10</f>
+        <v>400064000</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>